<commit_message>
overwriting player settings from command line
</commit_message>
<xml_diff>
--- a/results/mcts_player.xlsx
+++ b/results/mcts_player.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>playout_depth=50, eval_function=num_cards_weighted, weighted_backprop=0</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>input variable</t>
+  </si>
+  <si>
+    <t>find_root_node</t>
   </si>
 </sst>
 </file>
@@ -91,6 +94,305 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>pts ratio</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>gra_w_pana!$B$6:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>gra_w_pana!$B$7:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.46635399999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48451699999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.47669699999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.47417799999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.47159200000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.47928100000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.43764700000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>found terminal node</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>gra_w_pana!$B$6:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>gra_w_pana!$B$8:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.42819443075676444</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41086394316925817</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.41539606592238171</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.37143533564341519</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.37813031034791161</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.31311890859968966</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.17987350994076717</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>found root node</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>gra_w_pana!$B$6:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>gra_w_pana!$B$9:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.83333333333333337</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82959641255605376</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84103512014787429</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.80135823429541597</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.65635451505016718</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.43296089385474862</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3758278145695364</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="56409472"/>
+        <c:axId val="56415360"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="56409472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56415360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="56415360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56409472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -390,7 +692,7 @@
     <col min="2" max="4" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -398,7 +700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -406,7 +708,7 @@
         <v>43809</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -414,7 +716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -422,7 +724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -430,53 +732,127 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6">
+        <v>2.5</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
         <v>1.5</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>0.5</v>
       </c>
+      <c r="G6">
+        <v>0.25</v>
+      </c>
+      <c r="H6">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7">
+        <v>0.46635399999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.48451699999999998</v>
+      </c>
+      <c r="D7">
         <v>0.47669699999999998</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>0.47417799999999999</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>0.47159200000000001</v>
       </c>
+      <c r="G7">
+        <v>0.47928100000000001</v>
+      </c>
+      <c r="H7">
+        <v>0.43764700000000001</v>
+      </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8">
-        <f>39068/54982</f>
-        <v>0.71055981957731618</v>
+        <f>39104/(52219+39104)</f>
+        <v>0.42819443075676444</v>
       </c>
       <c r="C8">
-        <f>34516/58410</f>
-        <v>0.59092621126519429</v>
+        <f>38288/(54901+38288)</f>
+        <v>0.41086394316925817</v>
       </c>
       <c r="D8">
-        <f>33823/55625</f>
-        <v>0.60805393258426965</v>
+        <f>39068/(54982+39068)</f>
+        <v>0.41539606592238171</v>
+      </c>
+      <c r="E8">
+        <f>34516/(58410+34516)</f>
+        <v>0.37143533564341519</v>
+      </c>
+      <c r="F8">
+        <f>33823/(55625+33823)</f>
+        <v>0.37813031034791161</v>
+      </c>
+      <c r="G8">
+        <f>28047/(61526+28047)</f>
+        <v>0.31311890859968966</v>
+      </c>
+      <c r="H8">
+        <f>17036/(77675+17036)</f>
+        <v>0.17987350994076717</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <f>900/(180+900)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C9">
+        <f>925/(190+925)</f>
+        <v>0.82959641255605376</v>
+      </c>
+      <c r="D9">
+        <f>910/(172+910)</f>
+        <v>0.84103512014787429</v>
+      </c>
+      <c r="E9">
+        <f>944/(234+944)</f>
+        <v>0.80135823429541597</v>
+      </c>
+      <c r="F9">
+        <f>785/(411+785)</f>
+        <v>0.65635451505016718</v>
+      </c>
+      <c r="G9">
+        <f>465/(609+465)</f>
+        <v>0.43296089385474862</v>
+      </c>
+      <c r="H9">
+        <f>454/(754+454)</f>
+        <v>0.3758278145695364</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>